<commit_message>
practice on feb 20th
</commit_message>
<xml_diff>
--- a/docs/algo basics.xlsx
+++ b/docs/algo basics.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aganagav\Documents\Interview\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aganagav\IdeaProjects\test\datastructures\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E61CE84-F2DF-471F-8BEC-50D224931294}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73305C81-1CE6-45A9-A9E2-FB84F485CB1E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="6" xr2:uid="{BEA63947-71AD-42D5-B37A-6E351286DDB3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" activeTab="6" xr2:uid="{BEA63947-71AD-42D5-B37A-6E351286DDB3}"/>
   </bookViews>
   <sheets>
     <sheet name="Approach" sheetId="4" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t xml:space="preserve">Arrays </t>
   </si>
@@ -597,6 +597,9 @@
   </si>
   <si>
     <t>Bytecode can be executed on any platform (OS) using JVM( Java Virtual Machine).</t>
+  </si>
+  <si>
+    <t>Used access the classes, method and veriales at runtime.</t>
   </si>
 </sst>
 </file>
@@ -1304,7 +1307,7 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
   </cols>
@@ -1314,7 +1317,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="115.2">
+    <row r="2" spans="1:1" ht="120">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1332,11 +1335,11 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="37.109375" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" customWidth="1"/>
-    <col min="7" max="7" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="49.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1">
@@ -1380,7 +1383,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="57.6">
+    <row r="3" spans="1:8" ht="60">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1393,7 +1396,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="100.8">
+    <row r="4" spans="1:8" ht="105">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1404,7 +1407,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:8" ht="57.6">
+    <row r="5" spans="1:8" ht="60">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1429,23 +1432,23 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="68.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="102.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="102.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="58.95" customHeight="1">
+    <row r="1" spans="1:2" ht="58.9" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="28.8">
+    <row r="3" spans="1:2" ht="30">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="69.599999999999994">
+    <row r="5" spans="1:2" ht="72">
       <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
@@ -1453,7 +1456,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="52.2">
+    <row r="6" spans="1:2" ht="72">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1475,15 +1478,15 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="79.6640625" customWidth="1"/>
-    <col min="2" max="2" width="51.88671875" customWidth="1"/>
+    <col min="1" max="1" width="79.7109375" customWidth="1"/>
+    <col min="2" max="2" width="51.85546875" customWidth="1"/>
     <col min="3" max="3" width="42" customWidth="1"/>
-    <col min="4" max="4" width="27.44140625" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="100.2" customHeight="1">
+    <row r="1" spans="1:4" ht="100.15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1513,7 +1516,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="115.2">
+    <row r="6" spans="1:4" ht="120">
       <c r="A6" s="1" t="s">
         <v>55</v>
       </c>
@@ -1527,7 +1530,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="82.2">
+    <row r="7" spans="1:4" ht="99">
       <c r="A7" s="8" t="s">
         <v>46</v>
       </c>
@@ -1547,7 +1550,7 @@
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="18" spans="1:15">
       <c r="A18" t="s">
@@ -1645,9 +1648,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="56.5546875" customWidth="1"/>
+    <col min="2" max="2" width="56.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1660,7 +1663,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="72">
+    <row r="3" spans="1:2" ht="75">
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1681,16 +1684,16 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.33203125" customWidth="1"/>
-    <col min="3" max="3" width="50.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.44140625" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" customWidth="1"/>
+    <col min="3" max="3" width="50.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" customWidth="1"/>
+    <col min="5" max="5" width="52.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1">
@@ -1710,7 +1713,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="72">
+    <row r="2" spans="1:5" ht="75">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1723,8 +1726,11 @@
       <c r="D2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="158.4">
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="180">
       <c r="B3" s="1" t="s">
         <v>30</v>
       </c>
@@ -1735,7 +1741,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="72">
+    <row r="4" spans="1:5" ht="75">
       <c r="B4" t="s">
         <v>32</v>
       </c>
@@ -1756,12 +1762,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="57.6">
+    <row r="7" spans="1:5" ht="60">
       <c r="C7" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="201.6">
+    <row r="8" spans="1:5" ht="210">
       <c r="C8" s="1" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
practice on feb 23th
</commit_message>
<xml_diff>
--- a/docs/algo basics.xlsx
+++ b/docs/algo basics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aganagav\IdeaProjects\test\datastructures\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73305C81-1CE6-45A9-A9E2-FB84F485CB1E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CEAB7D-5AA0-4F08-B107-46BD44948240}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" activeTab="6" xr2:uid="{BEA63947-71AD-42D5-B37A-6E351286DDB3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" activeTab="1" xr2:uid="{BEA63947-71AD-42D5-B37A-6E351286DDB3}"/>
   </bookViews>
   <sheets>
     <sheet name="Approach" sheetId="4" r:id="rId1"/>
@@ -192,15 +192,6 @@
 3. balanced parenthesses , {[]}</t>
   </si>
   <si>
-    <t>BlockingQueue
-ArrayBlockingQueue
-DelayQueue
-LinkedBlockingQueue
-PriorityBlockingQueue
-SynchronousQueue
-FIFO</t>
-  </si>
-  <si>
     <t>Method: EnQueue(x)
 DeQueue()
 Front()
@@ -600,6 +591,16 @@
   </si>
   <si>
     <t>Used access the classes, method and veriales at runtime.</t>
+  </si>
+  <si>
+    <t>BlockingQueue
+ArrayBlockingQueue
+DelayQueue
+LinkedBlockingQueue
+PriorityQueue
+PriorityBlockingQueue
+SynchronousQueue
+FIFO</t>
   </si>
 </sst>
 </file>
@@ -1331,8 +1332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8D4487-6604-4DF9-95AE-2E9BF77FAAB4}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1365,12 +1366,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="120">
+    <row r="2" spans="1:8" ht="135">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="5" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>20</v>
@@ -1388,7 +1389,7 @@
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>21</v>
@@ -1412,7 +1413,7 @@
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -1440,7 +1441,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="58.9" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30">
@@ -1450,18 +1451,18 @@
     </row>
     <row r="5" spans="1:2" ht="72">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="72">
       <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1504,35 +1505,35 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
         <v>49</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="120">
       <c r="A6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="99">
       <c r="A7" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1554,83 +1555,83 @@
   <sheetData>
     <row r="18" spans="1:15">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O23" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:15">
       <c r="O25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:15">
       <c r="O26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:15">
       <c r="O28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:15">
       <c r="O30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:15">
       <c r="O32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:16">
       <c r="O34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:16">
       <c r="O36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:16">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:16">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:16">
       <c r="P40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1683,7 +1684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEF77B21-21B8-40BC-9655-386975AB0181}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -1698,78 +1699,78 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="75">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="180">
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="75">
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="C5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="C6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="60">
       <c r="C7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="210">
       <c r="C8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>